<commit_message>
some column data copied
</commit_message>
<xml_diff>
--- a/College-Scorecard-Analysis/college-scorecard-transforms.xlsx
+++ b/College-Scorecard-Analysis/college-scorecard-transforms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deka_\Desktop\Testing\Program Playground\College-Scorecard-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05352E44-0114-48F0-8934-711D04088206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA44D5F-8B20-41B9-8ED2-4F52AB2DE062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="87">
   <si>
     <t>NAME OF DATA ELEMENT</t>
   </si>
@@ -64,6 +64,233 @@
   </si>
   <si>
     <t>UNITID</t>
+  </si>
+  <si>
+    <t>Institution name</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>autocomplete</t>
+  </si>
+  <si>
+    <t>fulltext</t>
+  </si>
+  <si>
+    <t>INSTNM</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>State postcode</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>STABBR</t>
+  </si>
+  <si>
+    <t>Flag for main campus</t>
+  </si>
+  <si>
+    <t>main_campus</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t>Not main campus</t>
+  </si>
+  <si>
+    <t>Main campus</t>
+  </si>
+  <si>
+    <t>Highest degree awarded
+ 0 Non-degree-granting
+ 1 Certificate degree
+ 2 Associate degree
+ 3 Bachelor's degree
+ 4 Graduate degree</t>
+  </si>
+  <si>
+    <t>degrees_awarded.highest</t>
+  </si>
+  <si>
+    <t>HIGHDEG</t>
+  </si>
+  <si>
+    <t>Non-degree-granting</t>
+  </si>
+  <si>
+    <t>Certificate degree</t>
+  </si>
+  <si>
+    <t>Associate degree</t>
+  </si>
+  <si>
+    <t>Bachelor's degree</t>
+  </si>
+  <si>
+    <t>Graduate degree</t>
+  </si>
+  <si>
+    <t>Control of institution</t>
+  </si>
+  <si>
+    <t>ownership</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Private nonprofit</t>
+  </si>
+  <si>
+    <t>Private for-profit</t>
+  </si>
+  <si>
+    <t>Region (IPEDS)</t>
+  </si>
+  <si>
+    <t>region_id</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>U.S. Service Schools</t>
+  </si>
+  <si>
+    <t>New England (CT, ME, MA, NH, RI, VT)</t>
+  </si>
+  <si>
+    <t>Mid East (DE, DC, MD, NJ, NY, PA)</t>
+  </si>
+  <si>
+    <t>Great Lakes (IL, IN, MI, OH, WI)</t>
+  </si>
+  <si>
+    <t>Plains (IA, KS, MN, MO, NE, ND, SD)</t>
+  </si>
+  <si>
+    <t>Southeast (AL, AR, FL, GA, KY, LA, MS, NC, SC, TN, VA, WV)</t>
+  </si>
+  <si>
+    <t>Southwest (AZ, NM, OK, TX)</t>
+  </si>
+  <si>
+    <t>Rocky Mountains (CO, ID, MT, UT, WY)</t>
+  </si>
+  <si>
+    <t>Far West (AK, CA, HI, NV, OR, WA)</t>
+  </si>
+  <si>
+    <t>Outlying Areas (AS, FM, GU, MH, MP, PR, PW, VI)</t>
+  </si>
+  <si>
+    <t>Locale of institution</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>LOCALE</t>
+  </si>
+  <si>
+    <t>City: Large (population of 250,000 or more)</t>
+  </si>
+  <si>
+    <t>City: Midsize (population of at least 100,000 but less than 250,000)</t>
+  </si>
+  <si>
+    <t>City: Small (population less than 100,000)</t>
+  </si>
+  <si>
+    <t>Suburb: Large (outside principal city, in urbanized area with population of 250,000 or more)</t>
+  </si>
+  <si>
+    <t>Suburb: Midsize (outside principal city, in urbanized area with population of at least 100,000 but less than 250,000)</t>
+  </si>
+  <si>
+    <t>Suburb: Small (outside principal city, in urbanized area with population less than 100,000)</t>
+  </si>
+  <si>
+    <t>Town: Fringe (in urban cluster up to 10 miles from an urbanized area)</t>
+  </si>
+  <si>
+    <t>Town: Distant (in urban cluster more than 10 miles and up to 35 miles from an urbanized area)</t>
+  </si>
+  <si>
+    <t>Town: Remote (in urban cluster more than 35 miles from an urbanized area)</t>
+  </si>
+  <si>
+    <t>Rural: Fringe (rural territory up to 5 miles from an urbanized area or up to 2.5 miles from an urban cluster)</t>
+  </si>
+  <si>
+    <t>Rural: Distant (rural territory more than 5 miles but up to 25 miles from an urbanized area or more than 2.5 and up to 10 miles from an urban cluster)</t>
+  </si>
+  <si>
+    <t>Rural: Remote (rural territory more than 25 miles from an urbanized area and more than 10 miles from an urban cluster)</t>
+  </si>
+  <si>
+    <t>Degree of urbanization of institution</t>
+  </si>
+  <si>
+    <t>degree_urbanization</t>
+  </si>
+  <si>
+    <t>LOCALE2</t>
+  </si>
+  <si>
+    <t>Large City (a central city of a CMSA or MSA, with the city having a population greater than or equal to 250,000)</t>
+  </si>
+  <si>
+    <t>Mid-Size City (a central city of a CMSA or MSA, with the city having a population less than 250,000)</t>
+  </si>
+  <si>
+    <t>Urban Fringe of a Large City (any territory within a CMSA or MSA of a Large City and defined as urban by the Census Bureau)</t>
+  </si>
+  <si>
+    <t>Urban Fringe of a Mid-Size City (any territory within a CMSA or MSA of a Mid-Size City and defined as urban by the Census Bureau)</t>
+  </si>
+  <si>
+    <t>Large Town (an incorporated place or Census-designated place with a population greater than or equal to 25,000 and located outside a CMSA or MSA)</t>
+  </si>
+  <si>
+    <t>Small Town (an incorporated place or Census-designated place with a population less than 25,000 and greater than or equal to 2,500 and located outside a CMSA or MSA)</t>
+  </si>
+  <si>
+    <t>Rural, Outside MSA (any territory designated as rural by the Census Bureau that is outside a CMSA or MSA of a Large or Mid-Size City)</t>
+  </si>
+  <si>
+    <t>Rural, Inside MSA (any territory designated as rural by the Census Bureau that is within a CMSA or MSA of a Large or Mid-Size City)</t>
   </si>
 </sst>
 </file>
@@ -390,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -403,7 +630,7 @@
     <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.90625" customWidth="1"/>
     <col min="8" max="8" width="46.453125" customWidth="1"/>
@@ -452,6 +679,599 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
+      <c r="H25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31">
+        <v>23</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35">
+        <v>41</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36">
+        <v>42</v>
+      </c>
+      <c r="H36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>43</v>
+      </c>
+      <c r="H37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45">
+        <v>8</v>
+      </c>
+      <c r="H45" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>